<commit_message>
BOM and doc edits
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\git\weed-puller\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E53684C4-B9CF-4616-9739-85B7AEB1725E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D88E2A7F-379E-4C17-ACCD-1F0395EEDB01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3630" yWindow="1575" windowWidth="21975" windowHeight="12150" xr2:uid="{5F43266E-66D5-4670-8FE1-6F1A7DF29865}"/>
+    <workbookView xWindow="3705" yWindow="1935" windowWidth="21975" windowHeight="12150" activeTab="1" xr2:uid="{5F43266E-66D5-4670-8FE1-6F1A7DF29865}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Models" sheetId="1" r:id="rId1"/>
+    <sheet name="Hardware" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="59">
   <si>
     <t>Qty</t>
   </si>
@@ -156,13 +157,74 @@
   </si>
   <si>
     <t>Twotrees 1.5A 42Ncm 60oz Nema 17 Stepper Motor, 1m Cable 42BYGH 38MM (17HS4401S)</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/dp/B07WPFQZQ1</t>
+  </si>
+  <si>
+    <t>Arduino Nano 33 IoT with Headers [ABX00032]</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/dp/B0758ZTS61</t>
+  </si>
+  <si>
+    <t>5pcs DROK 5v Step Down, DC 4.5-24V to 5V 3A</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/dp/B01MQGMOKI</t>
+  </si>
+  <si>
+    <t>Comments/DataSheet/Specs</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/dp/B01NALDSJ0</t>
+  </si>
+  <si>
+    <t>DROK Buck Converter 12v to 5v, 5A USB Voltage Regulator DC 9V-36V Step Down to DC 5V-5.3V 5.2V 3.5-6A Volt Transformer Power Supply Module for Phone Fast Charging</t>
+  </si>
+  <si>
+    <t>DROK LCD Screen DC Buck Converter Adjustable Voltage Regulator 12V 6V-32V to 1.5-32V 5A, LCD Screen Step Down Converter with USB Port and Protective Case</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/dp/B07JZ2GQJF</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>- https://store.arduino.cc/products/arduino-nano-33-iot-with-headers
+- https://mm.digikey.com/Volume0/opasdata/d220001/medias/docus/697/ABX00032_Web.pdf
+- https://docs.arduino.cc/hardware/nano-33-iot/#tech-specs
+- https://mm.digikey.com/Volume0/opasdata/d220001/medias/docus/697/ABX00032_Web.pdf
+- https://docs.arduino.cc/hardware/nano-33-iot/#tech-specs</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/dp/B0CMQCG3M8</t>
+  </si>
+  <si>
+    <t>15pcs 220uF 35V 8x12mm Electrolytic Capacitor 220 UF MFD 35 Volt 0.32x0.47in Aluminum Capacitors</t>
+  </si>
+  <si>
+    <t>100uF per stepper will work, but 25V is close to 20V Battery.  Use 35V instead…</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/dp/B0CYPVMK9J</t>
+  </si>
+  <si>
+    <t>6pcs ELEGOO Half Breadboard Kit (400 Points, 2 pairs of power rails)</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/dp/B07QXP4KVZ</t>
+  </si>
+  <si>
+    <t>630pcs BOJACK 0-to-1M Ohm 1% 1/4W (17 diff values) Metal Film Resistor Kit</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -182,6 +244,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -208,11 +278,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -548,10 +625,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3E4B7CE-7D18-4EB3-8368-B9ABC9195BD9}">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -560,7 +637,8 @@
     <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="53.140625" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="33" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="40.28515625" customWidth="1"/>
+    <col min="7" max="7" width="33" style="5" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="45.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -573,7 +651,7 @@
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="G1" s="4"/>
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -595,7 +673,7 @@
       <c r="F2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="4" t="s">
         <v>18</v>
       </c>
       <c r="H2" s="1" t="s">
@@ -621,7 +699,7 @@
       <c r="F3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="5" t="s">
         <v>20</v>
       </c>
       <c r="H3" t="s">
@@ -662,187 +740,368 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{260CCA48-0DA7-4121-A4A6-68E38B826DB4}">
+  <dimension ref="A1:G19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="40.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="64.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="G1" s="5"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G2" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>14</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C13" si="0">B3*A3</f>
+        <v>28</v>
+      </c>
+      <c r="D3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="5"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="5"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="5"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <f>B7*A7</f>
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>53</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G7" s="5"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>11</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="D9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="5"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>16</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="D10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G10" s="5"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>20</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="D11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" s="5"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B12">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C12">
-        <f>B12*A12</f>
-        <v>28</v>
+        <f t="shared" si="0"/>
+        <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="G12" s="5"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B13">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C13">
-        <f>B13*A13</f>
-        <v>12</v>
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
       <c r="D13" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="G13" s="5"/>
+    </row>
+    <row r="14" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1</v>
       </c>
       <c r="B14">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="C14">
         <f>B14*A14</f>
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="D14" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1</v>
       </c>
       <c r="B15">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C15">
-        <f>B15*A15</f>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D15" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>1</v>
-      </c>
-      <c r="B16">
-        <v>8</v>
-      </c>
-      <c r="C16">
-        <f>B16*A16</f>
-        <v>8</v>
-      </c>
-      <c r="D16" t="s">
-        <v>35</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="G15" s="5"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F16" s="3" t="s">
-        <v>28</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="G16" s="5"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1</v>
       </c>
       <c r="B17">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C17">
         <f>B17*A17</f>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D17" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>1</v>
-      </c>
-      <c r="B18">
-        <v>16</v>
-      </c>
-      <c r="C18">
-        <f>B18*A18</f>
-        <v>16</v>
-      </c>
       <c r="D18" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>1</v>
-      </c>
-      <c r="B19">
-        <v>20</v>
-      </c>
-      <c r="C19">
-        <f>B19*A19</f>
-        <v>20</v>
-      </c>
-      <c r="D19" t="s">
-        <v>33</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>32</v>
+      <c r="F19" s="7" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F16" r:id="rId1" xr:uid="{FB60736F-5D7E-418E-B449-4DE935FB7095}"/>
-    <hyperlink ref="F15" r:id="rId2" xr:uid="{5EE38EFA-C9AD-4993-8A63-338679B98AB3}"/>
-    <hyperlink ref="F14" r:id="rId3" xr:uid="{5A737309-EAF5-4C13-963C-E2F2CDC45472}"/>
-    <hyperlink ref="F13" r:id="rId4" xr:uid="{78A732B2-A7D4-455C-B653-6664D62F8200}"/>
-    <hyperlink ref="F12" r:id="rId5" xr:uid="{C05A4A42-CBDB-4BFB-B886-AF5071371CA6}"/>
-    <hyperlink ref="F17" r:id="rId6" xr:uid="{31C0ACC0-01D2-419C-A773-08F30CBF53B6}"/>
-    <hyperlink ref="F18" r:id="rId7" xr:uid="{83B265F1-14DD-4F31-8FBA-6E018A88851D}"/>
-    <hyperlink ref="F19" r:id="rId8" xr:uid="{D265D09D-5549-4EAD-8DD5-B504F6C7E63F}"/>
+    <hyperlink ref="F8" r:id="rId1" xr:uid="{FB60736F-5D7E-418E-B449-4DE935FB7095}"/>
+    <hyperlink ref="F6" r:id="rId2" xr:uid="{5EE38EFA-C9AD-4993-8A63-338679B98AB3}"/>
+    <hyperlink ref="F5" r:id="rId3" xr:uid="{5A737309-EAF5-4C13-963C-E2F2CDC45472}"/>
+    <hyperlink ref="F4" r:id="rId4" xr:uid="{78A732B2-A7D4-455C-B653-6664D62F8200}"/>
+    <hyperlink ref="F3" r:id="rId5" xr:uid="{C05A4A42-CBDB-4BFB-B886-AF5071371CA6}"/>
+    <hyperlink ref="F9" r:id="rId6" xr:uid="{31C0ACC0-01D2-419C-A773-08F30CBF53B6}"/>
+    <hyperlink ref="F10" r:id="rId7" xr:uid="{83B265F1-14DD-4F31-8FBA-6E018A88851D}"/>
+    <hyperlink ref="F11" r:id="rId8" xr:uid="{D265D09D-5549-4EAD-8DD5-B504F6C7E63F}"/>
+    <hyperlink ref="F14" r:id="rId9" xr:uid="{758B0787-BF06-43D0-8184-E2F9033F2EF4}"/>
+    <hyperlink ref="G14" r:id="rId10" display="https://mm.digikey.com/Volume0/opasdata/d220001/medias/docus/697/ABX00032_Web.pdf" xr:uid="{B47394E6-187E-46F5-91DE-A70D9A48E97E}"/>
+    <hyperlink ref="F15" r:id="rId11" xr:uid="{84864E26-FBE2-4A58-A732-1D9F5CDD153C}"/>
+    <hyperlink ref="F16" r:id="rId12" xr:uid="{2C0501DA-5A3D-4D3C-9A74-36AB9665A23E}"/>
+    <hyperlink ref="F17" r:id="rId13" xr:uid="{2416265F-24DC-433B-80A9-DA1D1BF817E4}"/>
+    <hyperlink ref="F18" r:id="rId14" xr:uid="{4CAEDABD-3583-4B2F-A49E-C81020803D07}"/>
+    <hyperlink ref="F7" r:id="rId15" xr:uid="{CB29767D-028B-4800-A925-687F7DC4209D}"/>
+    <hyperlink ref="F12" r:id="rId16" xr:uid="{568CB923-AD5B-475D-8D35-C25AFF0CA08E}"/>
+    <hyperlink ref="F13" r:id="rId17" xr:uid="{CE88AF18-4B15-4427-B0DF-62BC3404057C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId9"/>
+  <pageSetup orientation="portrait" r:id="rId18"/>
 </worksheet>
 </file>
</xml_diff>